<commit_message>
Update resume and linkedin links on wiki
</commit_message>
<xml_diff>
--- a/iGEM_Links.xlsx
+++ b/iGEM_Links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omar/Desktop/iGEM_2019/wiki/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3654DDCE-FD72-8941-9B70-822D4D035E42}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70604D6-C0A0-A247-9F33-79F9F16F5CF0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" activeTab="4" xr2:uid="{4C17A8AC-393A-4CA5-94E7-54FFA60CB45B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" activeTab="5" xr2:uid="{4C17A8AC-393A-4CA5-94E7-54FFA60CB45B}"/>
   </bookViews>
   <sheets>
     <sheet name="CSS" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="180">
   <si>
     <t>https://2019.igem.org/Team:CMUQ/components</t>
   </si>
@@ -1441,7 +1441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C77720-AE95-4068-B6DE-4C0C0BC0D6AD}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -1926,8 +1926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21A276B-EBB5-431B-A41D-C0AB0D8FD621}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1994,9 +1994,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>84</v>
-      </c>
+      <c r="A8" s="11"/>
       <c r="B8" s="10" t="s">
         <v>73</v>
       </c>
@@ -2048,16 +2046,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1" xr:uid="{2BF8B63B-2DA7-45B0-AEDA-0000EF79462D}"/>
-    <hyperlink ref="A9" r:id="rId2" xr:uid="{688D4C0D-8EBD-488D-AC40-F955406F45F5}"/>
-    <hyperlink ref="A6" r:id="rId3" xr:uid="{575B705B-0892-4489-B6BF-50D36D8D2438}"/>
-    <hyperlink ref="A2" r:id="rId4" xr:uid="{283E196A-709A-4A19-91A4-B708EEC51BFC}"/>
-    <hyperlink ref="A3" r:id="rId5" xr:uid="{11FF0A93-982C-4A78-8013-B1FB0ED077D6}"/>
-    <hyperlink ref="A4" r:id="rId6" xr:uid="{33E5F4DD-6C42-4C96-AA4E-382241C5AA87}"/>
-    <hyperlink ref="A5" r:id="rId7" xr:uid="{FF26779B-21C8-4D47-919D-0880271C6248}"/>
-    <hyperlink ref="A7" r:id="rId8" xr:uid="{8CB7173F-30DE-4DA0-B127-F27B1CC22DE7}"/>
-    <hyperlink ref="A10" r:id="rId9" xr:uid="{673EDDEF-2BB6-470B-AE4A-6E6E6A1EE11B}"/>
-    <hyperlink ref="A14" r:id="rId10" xr:uid="{F30B6B40-F221-409A-A82C-DBBF106DBF6D}"/>
+    <hyperlink ref="A9" r:id="rId1" xr:uid="{688D4C0D-8EBD-488D-AC40-F955406F45F5}"/>
+    <hyperlink ref="A6" r:id="rId2" xr:uid="{575B705B-0892-4489-B6BF-50D36D8D2438}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{283E196A-709A-4A19-91A4-B708EEC51BFC}"/>
+    <hyperlink ref="A3" r:id="rId4" xr:uid="{11FF0A93-982C-4A78-8013-B1FB0ED077D6}"/>
+    <hyperlink ref="A4" r:id="rId5" xr:uid="{33E5F4DD-6C42-4C96-AA4E-382241C5AA87}"/>
+    <hyperlink ref="A5" r:id="rId6" xr:uid="{FF26779B-21C8-4D47-919D-0880271C6248}"/>
+    <hyperlink ref="A7" r:id="rId7" xr:uid="{8CB7173F-30DE-4DA0-B127-F27B1CC22DE7}"/>
+    <hyperlink ref="A10" r:id="rId8" xr:uid="{673EDDEF-2BB6-470B-AE4A-6E6E6A1EE11B}"/>
+    <hyperlink ref="A14" r:id="rId9" xr:uid="{F30B6B40-F221-409A-A82C-DBBF106DBF6D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2068,7 +2065,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update links for materialize
</commit_message>
<xml_diff>
--- a/iGEM_Links.xlsx
+++ b/iGEM_Links.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omar/Desktop/iGEM_2019/wiki/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omar/Documents/iGEM_2019/wiki/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70604D6-C0A0-A247-9F33-79F9F16F5CF0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6666D705-98CF-DA48-8B5F-842100CDA70D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" activeTab="5" xr2:uid="{4C17A8AC-393A-4CA5-94E7-54FFA60CB45B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" xr2:uid="{4C17A8AC-393A-4CA5-94E7-54FFA60CB45B}"/>
   </bookViews>
   <sheets>
     <sheet name="CSS" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="185">
   <si>
     <t>https://2019.igem.org/Team:CMUQ/components</t>
   </si>
@@ -571,6 +571,21 @@
   </si>
   <si>
     <t>linkedin logo</t>
+  </si>
+  <si>
+    <t>https://2019.igem.org/wiki/images/3/3b/T--CMUQ--wikijoanaresume.pdf</t>
+  </si>
+  <si>
+    <t>materialize.css</t>
+  </si>
+  <si>
+    <t>https://2019.igem.org/wiki/index.php?title=Team:CMUQ/materialize-css&amp;action=raw&amp;ctype=text/css</t>
+  </si>
+  <si>
+    <t>materialize.js</t>
+  </si>
+  <si>
+    <t>https://2019.igem.org/wiki/index.php?title=Team:CMUQ/materialize-js&amp;action=raw&amp;ctype=text/javascript</t>
   </si>
 </sst>
 </file>
@@ -1019,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D80558-3075-45B9-9436-5060B6533359}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1086,6 +1101,22 @@
       </c>
       <c r="C6" s="2"/>
     </row>
+    <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A5" r:id="rId1" xr:uid="{11152AD3-3997-4986-B427-B3BD3563B8A9}"/>
@@ -1093,9 +1124,11 @@
     <hyperlink ref="A4" r:id="rId3" xr:uid="{C43A25CE-33A2-453F-A66F-208B6CDC840D}"/>
     <hyperlink ref="A3" r:id="rId4" xr:uid="{F54ED7CA-0829-4E25-A6DF-64A3BBCA642E}"/>
     <hyperlink ref="A2" r:id="rId5" xr:uid="{40DB5EE2-F92C-4368-9596-F24D06E49A76}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{7DDBC47B-E78B-3D43-8EE3-A656D954DB54}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{BE155BDF-1368-B345-9E0B-69A4B3A6C028}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -1926,8 +1959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21A276B-EBB5-431B-A41D-C0AB0D8FD621}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2028,7 +2061,9 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="11" t="s">
+        <v>180</v>
+      </c>
       <c r="B13" s="5" t="s">
         <v>80</v>
       </c>
@@ -2055,6 +2090,7 @@
     <hyperlink ref="A7" r:id="rId7" xr:uid="{8CB7173F-30DE-4DA0-B127-F27B1CC22DE7}"/>
     <hyperlink ref="A10" r:id="rId8" xr:uid="{673EDDEF-2BB6-470B-AE4A-6E6E6A1EE11B}"/>
     <hyperlink ref="A14" r:id="rId9" xr:uid="{F30B6B40-F221-409A-A82C-DBBF106DBF6D}"/>
+    <hyperlink ref="A13" r:id="rId10" xr:uid="{477619E7-EA82-F949-B623-3E4073D054AF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update lab notebook links
</commit_message>
<xml_diff>
--- a/iGEM_Links.xlsx
+++ b/iGEM_Links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omar/Documents/iGEM_2019/wiki/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12933549-14B7-944B-8037-CF96CE011CA9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF04635-1F2D-0641-85C8-B229C2D1FE33}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" activeTab="4" xr2:uid="{4C17A8AC-393A-4CA5-94E7-54FFA60CB45B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="211">
   <si>
     <t>https://2019.igem.org/Team:CMUQ/components</t>
   </si>
@@ -625,6 +625,45 @@
   </si>
   <si>
     <t>https://2019.igem.org/wiki/images/9/9b/T--CMUQ--wikiimgqf.png</t>
+  </si>
+  <si>
+    <t>https://2019.igem.org/wiki/images/8/84/T--CMUQ--notebook-15052019-1.png</t>
+  </si>
+  <si>
+    <t>notebook-15052019-1.png</t>
+  </si>
+  <si>
+    <t>Lab Notebook</t>
+  </si>
+  <si>
+    <t>https://2019.igem.org/wiki/images/5/52/T--CMUQ--notebook-15052019.png</t>
+  </si>
+  <si>
+    <t>notebook-15052019.png</t>
+  </si>
+  <si>
+    <t>https://2019.igem.org/wiki/images/thumb/b/b6/T--CMUQ--notebook-16052019-1.jpg/800px-T--CMUQ--notebook-16052019-1.jpg</t>
+  </si>
+  <si>
+    <t>notebook-16052019-1.jpg</t>
+  </si>
+  <si>
+    <t>https://2019.igem.org/wiki/images/thumb/a/a6/T--CMUQ--notebook-16052019.jpg/450px-T--CMUQ--notebook-16052019.jpg</t>
+  </si>
+  <si>
+    <t>notebook-16052019.jpg</t>
+  </si>
+  <si>
+    <t>https://2019.igem.org/wiki/images/b/be/T--CMUQ--notebook-23052019-1.png</t>
+  </si>
+  <si>
+    <t>notebook-23052019-1.png</t>
+  </si>
+  <si>
+    <t>https://2019.igem.org/wiki/images/thumb/6/6b/T--CMUQ--notebook-23052019.png/713px-T--CMUQ--notebook-23052019.png</t>
+  </si>
+  <si>
+    <t>notebook-23052019.png</t>
   </si>
 </sst>
 </file>
@@ -1529,10 +1568,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C77720-AE95-4068-B6DE-4C0C0BC0D6AD}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1991,12 +2030,96 @@
         <v>131</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>134</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B35" t="s">
+        <v>199</v>
+      </c>
+      <c r="C35" t="s">
+        <v>200</v>
+      </c>
+      <c r="E35" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B36" t="s">
+        <v>202</v>
+      </c>
+      <c r="C36" t="s">
+        <v>200</v>
+      </c>
+      <c r="E36" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B37" t="s">
+        <v>204</v>
+      </c>
+      <c r="C37" t="s">
+        <v>200</v>
+      </c>
+      <c r="E37" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B38" t="s">
+        <v>206</v>
+      </c>
+      <c r="C38" t="s">
+        <v>200</v>
+      </c>
+      <c r="E38" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B39" t="s">
+        <v>208</v>
+      </c>
+      <c r="C39" t="s">
+        <v>200</v>
+      </c>
+      <c r="E39" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B40" t="s">
+        <v>210</v>
+      </c>
+      <c r="C40" t="s">
+        <v>200</v>
+      </c>
+      <c r="E40" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2026,6 +2149,12 @@
     <hyperlink ref="A25" r:id="rId23" xr:uid="{6DB402F7-C9CA-834E-9872-713ABC69D423}"/>
     <hyperlink ref="A27" r:id="rId24" xr:uid="{832E807A-D19D-2541-8BFE-2B75DC054159}"/>
     <hyperlink ref="A32" r:id="rId25" xr:uid="{DD0FBBAE-B902-7E4B-BFE6-C6E0DAF327C2}"/>
+    <hyperlink ref="A35" r:id="rId26" xr:uid="{1B417A74-41F4-3B47-9C6C-51477755DD36}"/>
+    <hyperlink ref="A36" r:id="rId27" xr:uid="{E778FE6C-93B4-5B46-AD9E-B07B553E983A}"/>
+    <hyperlink ref="A37" r:id="rId28" xr:uid="{ADEC864B-437B-C347-8BAC-84124CCEFCC4}"/>
+    <hyperlink ref="A38" r:id="rId29" xr:uid="{7A0EB37E-0C66-2544-89FF-6B7F9F3862DB}"/>
+    <hyperlink ref="A39" r:id="rId30" xr:uid="{7F0553E1-91A3-0D48-8D5A-785F8C09D2EA}"/>
+    <hyperlink ref="A40" r:id="rId31" xr:uid="{2D02BCDF-6E8B-7142-A6B6-422032DCE1D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>